<commit_message>
add changes tables and changes graphs
</commit_message>
<xml_diff>
--- a/falla_frecuencia.xlsx
+++ b/falla_frecuencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos GitHub\PYTHON-PANDAS-ALGORITM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7511A32C-C797-4354-BE93-E9EE3713E365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F263F86-2FEA-4D80-BCDA-4DC91A02F0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1965" yWindow="0" windowWidth="18525" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Format</t>
   </si>
@@ -157,7 +157,10 @@
     <t>TIEMPO</t>
   </si>
   <si>
-    <t>Waveform Data 1</t>
+    <t>WaveformData</t>
+  </si>
+  <si>
+    <t>WaveformData1</t>
   </si>
 </sst>
 </file>
@@ -14255,7 +14258,7 @@
   <dimension ref="A1:F1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14268,10 +14271,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>29</v>

</xml_diff>